<commit_message>
Program is ready to download all corpuses
</commit_message>
<xml_diff>
--- a/input_data/subreddit-corpus.xlsx
+++ b/input_data/subreddit-corpus.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,17 +458,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>4keu48</t>
+          <t>30pk7l</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>[deleted]</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -478,17 +474,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4kev7e</t>
+          <t>58ccmp</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>[deleted]</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -498,17 +490,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4kevqg</t>
+          <t>39nogp</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>[deleted]</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -518,27 +506,23 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4kew87</t>
+          <t>39nogp</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[deleted]</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+          <t>Sggvgcjcjvgc</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4kewo5</t>
+          <t>77swzz</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -558,17 +542,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4kewxz</t>
+          <t>2s8qgt</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>[deleted]</t>
-        </is>
-      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -578,18 +558,146 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4kfafh</t>
+          <t>63uwn9</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>6uuo26</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>RAID THIS he hurt me today</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>6x3ygl</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>After making all these I got a feel for what I liked and didn't, so juuuust for fun, Here are some awards - don't @ me.Bonus awards_____________Best Logo : San Jose SharksRunner up : Florida PanthersMost creative logo : Minnesota WildRunner up : Colorado AvalancheBest colors : Edmonton OilersRunner up : Arizona CoyotesWorst logo : Carolina HurricanesRunner up : Las Vegas Golden KnightsWorst colors : Las Vegas Golden KnightsRunner up : New Jersey DevilsBest alternate/retro logo : Anaheim DucksRunner up : Calgary FlamesMost creative alternate/retro logo : Arizona (Pheonix) CoyotesRunner up : Detroit Red WingsWorst alternate/retro logo : Ottawa SenatorsRunner up : Los Angeles Kings</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>6x3ygl</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>[deleted]</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>After making all these I got a feel for what I liked and didn't, so juuuust for fun, Here are some awards - don't @ me.Bonus awards_____________Best Logo : San Jose SharksRunner up : Florida PanthersMost creative logo : Minnesota WildRunner up : Colorado AvalancheBest colors : Edmonton OilersRunner up : Arizona CoyotesWorst logo : Carolina HurricanesRunner up : Las Vegas Golden KnightsWorst colors : Las Vegas Golden KnightsRunner up : New Jersey DevilsBest alternate/retro logo : Anaheim DucksRunner up : Calgary FlamesMost creative alternate/retro logo : Arizona (Pheonix) CoyotesRunner up : Detroit Red WingsWorst alternate/retro logo : Ottawa SenatorsRunner up : Los Angeles Kings</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>6x3ygl</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>[deleted]</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>After making all these I got a feel for what I liked and didn't, so juuuust for fun, Here are some awards - don't @ me.Bonus awards_____________Best Logo : San Jose SharksRunner up : Florida PanthersMost creative logo : Minnesota WildRunner up : Colorado AvalancheBest colors : Edmonton OilersRunner up : Arizona CoyotesWorst logo : Carolina HurricanesRunner up : Las Vegas Golden KnightsWorst colors : Las Vegas Golden KnightsRunner up : New Jersey DevilsBest alternate/retro logo : Anaheim DucksRunner up : Calgary FlamesMost creative alternate/retro logo : Arizona (Pheonix) CoyotesRunner up : Detroit Red WingsWorst alternate/retro logo : Ottawa SenatorsRunner up : Los Angeles Kings</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>6x3ygl</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>It’s-a-me, Mario, and I love lasagna!</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>[deleted]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>3qcw3c</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>6eu2g1</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>